<commit_message>
Risolto consuntivo PDROP nel PP
</commit_message>
<xml_diff>
--- a/Documents/RA/ExternalDocuments/PianoDiProgetto/consuntivi/consuntivo.xlsx
+++ b/Documents/RA/ExternalDocuments/PianoDiProgetto/consuntivi/consuntivo.xlsx
@@ -4275,7 +4275,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:numFmt formatCode="&quot;€ &quot;#,##0.00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4307,9 +4306,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-B8F5-4B74-9221-990DC78BCFB6}"/>
                 </c:ext>
@@ -10388,7 +10385,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
-              <c:layout/>
               <c:numFmt formatCode="&quot;€ &quot;#,##0.00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -10420,9 +10416,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-6A14-452F-9341-30D4AA8265C4}"/>
                 </c:ext>
@@ -14534,13 +14528,13 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>176</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>300</c:v>
@@ -15171,13 +15165,13 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>20</c:v>
@@ -32867,8 +32861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33406,20 +33400,20 @@
         <v>16</v>
       </c>
       <c r="D39" s="17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E39" s="18">
         <v>10</v>
       </c>
       <c r="F39" s="17">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G39" s="18">
         <v>20</v>
       </c>
       <c r="H39" s="19">
         <f>B39+C39+D39+E39+F39+G39</f>
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33518,11 +33512,11 @@
       </c>
       <c r="C46" s="39">
         <f>D$39-B46</f>
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="D46" s="39">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E46" s="23">
         <f t="shared" si="2"/>
@@ -33530,11 +33524,11 @@
       </c>
       <c r="F46" s="23">
         <f>(C46*22)</f>
-        <v>-176</v>
+        <v>-132</v>
       </c>
       <c r="G46" s="23">
         <f>(D46*22)</f>
-        <v>176</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33576,11 +33570,11 @@
       </c>
       <c r="C48" s="39">
         <f>F$39-B48</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D48" s="39">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E48" s="23">
         <f t="shared" si="2"/>
@@ -33588,11 +33582,11 @@
       </c>
       <c r="F48" s="23">
         <f>(C48*15)</f>
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="G48" s="23">
         <f>(D48*15)</f>
-        <v>300</v>
+        <v>345</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33634,11 +33628,11 @@
       </c>
       <c r="C50" s="40">
         <f>H39-B50</f>
-        <v>-14</v>
+        <v>-9</v>
       </c>
       <c r="D50" s="40">
         <f>SUM(D44:D49)</f>
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E50" s="41">
         <f t="shared" si="2"/>
@@ -33646,11 +33640,11 @@
       </c>
       <c r="F50" s="28">
         <f>SUM(F44:F49)</f>
-        <v>-421</v>
+        <v>-332</v>
       </c>
       <c r="G50" s="28">
         <f>SUM(G44:G49)</f>
-        <v>1556</v>
+        <v>1645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>